<commit_message>
Changed wording of SParameters from 'Reflection, Gain, ...' to S11, S21, ... Also started building unit tests for plot generation: TraceSettingsTest, MeasureDataTest and ProcessTraceTest. TraceSettingsTest is finished, the others are still in early stages.
</commit_message>
<xml_diff>
--- a/Documentation/TracePermutations.xlsx
+++ b/Documentation/TracePermutations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="8970" windowHeight="4995"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="8970" windowHeight="4995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>Y</t>
   </si>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,10 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -545,20 +548,28 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>4</v>
       </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cross checked and improved comments for Documentation/TracePermutations.xlsx and UnitTests/TraceSettingsTest.cpp
</commit_message>
<xml_diff>
--- a/Documentation/TracePermutations.xlsx
+++ b/Documentation/TracePermutations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>Y</t>
   </si>
@@ -69,7 +69,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +79,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -106,9 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +422,7 @@
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
@@ -420,7 +439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -436,8 +455,11 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -445,7 +467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -453,7 +475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -470,7 +492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -487,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -501,32 +523,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -543,7 +563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -551,7 +571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -559,7 +579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>12</v>
       </c>

</xml_diff>